<commit_message>
add concurrent therapies to table
</commit_message>
<xml_diff>
--- a/exploratory/data/terminated_ongoing_trials_tabledata.xlsx
+++ b/exploratory/data/terminated_ongoing_trials_tabledata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahbukovac/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971A9EF1-ABC0-B248-B0E9-9E6B3931A890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550F1BFB-0F6B-104A-B243-641DEECC5FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="2640" windowWidth="34200" windowHeight="20160" xr2:uid="{C471BA0F-17ED-754C-92C2-4D7A276D29CD}"/>
+    <workbookView xWindow="840" yWindow="7860" windowWidth="34200" windowHeight="20160" xr2:uid="{C471BA0F-17ED-754C-92C2-4D7A276D29CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="87">
   <si>
     <t>Trial ID</t>
   </si>
@@ -267,6 +267,36 @@
   </si>
   <si>
     <t>Trial Initiation</t>
+  </si>
+  <si>
+    <t>Adjuvant Therapy</t>
+  </si>
+  <si>
+    <t>Immunotherapy</t>
+  </si>
+  <si>
+    <t>Chemoradiation</t>
+  </si>
+  <si>
+    <t>Androgen deprivation therapy</t>
+  </si>
+  <si>
+    <t>Chemotherapy</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Chemo and/or Radiation therapy</t>
+  </si>
+  <si>
+    <t>(SOC endocrine therapy and SGLT2i Therapy) or PI3K inhibition</t>
+  </si>
+  <si>
+    <t>Stereotactic radiosurgery</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -660,15 +690,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEFA523A-E0B2-914C-A34A-82FB427E6A42}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,8 +717,11 @@
       <c r="F1" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -707,8 +740,11 @@
       <c r="F2">
         <v>2025</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -727,8 +763,11 @@
       <c r="F3">
         <v>2025</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -747,8 +786,11 @@
       <c r="F4">
         <v>2020</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -767,8 +809,11 @@
       <c r="F5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -787,8 +832,11 @@
       <c r="F6">
         <v>2011</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -807,8 +855,11 @@
       <c r="F7">
         <v>2009</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -827,8 +878,11 @@
       <c r="F8">
         <v>2022</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -847,8 +901,11 @@
       <c r="F9">
         <v>2012</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -867,8 +924,11 @@
       <c r="F10">
         <v>2017</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -887,8 +947,11 @@
       <c r="F11">
         <v>2023</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -907,8 +970,11 @@
       <c r="F12">
         <v>2023</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -927,8 +993,11 @@
       <c r="F13">
         <v>2024</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -947,8 +1016,11 @@
       <c r="F14">
         <v>2011</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -967,8 +1039,11 @@
       <c r="F15">
         <v>2018</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -987,8 +1062,11 @@
       <c r="F16">
         <v>2023</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1007,8 +1085,11 @@
       <c r="F17">
         <v>2013</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1027,8 +1108,11 @@
       <c r="F18">
         <v>2014</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1047,8 +1131,11 @@
       <c r="F19">
         <v>2021</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1067,8 +1154,11 @@
       <c r="F20">
         <v>2022</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1087,8 +1177,11 @@
       <c r="F21">
         <v>2024</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1107,8 +1200,11 @@
       <c r="F22">
         <v>2022</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1127,8 +1223,11 @@
       <c r="F23">
         <v>2018</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1146,6 +1245,9 @@
       </c>
       <c r="F24">
         <v>2018</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>